<commit_message>
update and lot to drop
</commit_message>
<xml_diff>
--- a/Modelos_Campos.xlsx
+++ b/Modelos_Campos.xlsx
@@ -20,10 +20,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="x_linea" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="x_subninea" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="x_fabricante" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.picking.type" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.picking" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.warehouse.orderpoint" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.quant" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.move" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.move.line" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.picking.type" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.picking" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.warehouse.orderpoint" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stock.quant" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="account.move" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="account.move.line" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -788,6 +792,13 @@
       <c r="A48" t="inlineStr">
         <is>
           <t>sale_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>x_studio_integer_field_3JL6M</t>
         </is>
       </c>
     </row>
@@ -1379,7 +1390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1674,12 +1685,1142 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>x_color</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A103"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>priority</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>date_deadline</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>company_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>product_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>description_picking</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>product_qty</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>product_uom_qty</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>product_uom</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>product_uom_category_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>product_tmpl_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>location_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>location_dest_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>partner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>move_dest_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>move_orig_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>picking_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>price_unit</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>procure_method</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>scrapped</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>scrap_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>group_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>rule_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>propagate_cancel</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>delay_alert_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>picking_type_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>is_inventory</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>move_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>move_line_nosuggest_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>origin_returned_move_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>returned_move_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>reserved_availability</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>restrict_partner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>route_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>warehouse_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>has_tracking</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>quantity_done</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>show_operations</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>picking_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>show_details_visible</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>show_reserved_availability</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>product_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>is_locked</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>is_initial_demand_editable</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>is_quantity_done_editable</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>reference</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>move_lines_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>package_level_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>picking_type_entire_packs</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>display_assign_serial</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>next_serial</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>next_serial_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>orderpoint_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>forecast_availability</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>forecast_expected_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>lot_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>reservation_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>product_packaging_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>from_immediate_transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>__last_update</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>display_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>create_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>create_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>write_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>write_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>created_production_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>production_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>raw_material_production_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>unbuild_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>consume_unbuild_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>allowed_operation_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>operation_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>workorder_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>bom_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>byproduct_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>unit_factor</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>is_done</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>order_finished_lot_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>should_consume_qty</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>cost_share</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>product_qty_available</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>product_virtual_available</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>description_bom_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>use_expiration_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>to_refund</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>account_move_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>stock_valuation_layer_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>analytic_account_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>purchase_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>created_purchase_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>created_purchase_request_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>purchase_request_allocation_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>purchase_request_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>requisition_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>sale_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>picking_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>move_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>company_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>product_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>product_uom_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>product_uom_category_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>product_qty</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>product_uom_qty</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>qty_done</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>package_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>package_level_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>lot_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>lot_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>result_package_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>owner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>location_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>location_dest_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>lots_visible</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>picking_partner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>picking_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>picking_type_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>picking_type_use_create_lots</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>picking_type_use_existing_lots</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>picking_type_entire_packs</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>is_initial_demand_editable</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>is_inventory</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>is_locked</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>consume_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>produce_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>reference</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>tracking</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>description_picking</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>__last_update</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>display_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>create_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>create_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>write_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>write_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>workorder_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>production_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>description_bom_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>expiration_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>sale_price</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>destination_country_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>carrier_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>x_studio_descripcin</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>x_studio_n_factura</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>x_studio_related_field_G1Fv7</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1971,7 +3112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2732,7 +3873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2996,7 +4137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3259,7 +4400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A121"/>
+  <dimension ref="A1:A124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4111,6 +5252,2018 @@
       <c r="A121" t="inlineStr">
         <is>
           <t>x_studio_related_field_K89Oj</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>x_studio_many2many_field_UhyOD</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>x_studio_many2many_field_iWTMQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>x_studio_many2many_field_YoTvr</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A191"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>campaign_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>source_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>medium_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sequence_prefix</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sequence_number</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>activity_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>activity_state</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>activity_user_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>activity_type_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>activity_type_icon</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>activity_date_deadline</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>my_activity_date_deadline</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>activity_summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>activity_exception_decoration</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>activity_exception_icon</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>activity_calendar_event_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>message_is_follower</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>message_follower_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>message_partner_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>message_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>has_message</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>message_unread</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>message_unread_counter</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>message_needaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>message_needaction_counter</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>message_has_error</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>message_has_error_counter</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>message_attachment_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>message_main_attachment_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>website_message_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>message_has_sms_error</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>access_url</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>access_token</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>access_warning</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>highest_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>show_name_warning</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>narration</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>posted_before</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>move_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>type_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>to_check</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>journal_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>suitable_journal_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>company_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>company_currency_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>currency_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>partner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>commercial_partner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>country_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>is_move_sent</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>partner_bank_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>payment_reference</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>payment_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>statement_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>statement_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>amount_untaxed</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>amount_tax</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>amount_total</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>amount_residual</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>amount_untaxed_signed</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>amount_tax_signed</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>amount_total_signed</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>amount_total_in_currency_signed</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>amount_residual_signed</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>tax_totals_json</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>payment_state</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>tax_cash_basis_rec_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>tax_cash_basis_origin_move_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>tax_cash_basis_created_move_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>always_tax_exigible</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>auto_post</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>reversed_entry_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>reversal_move_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>fiscal_position_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>invoice_user_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>invoice_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>invoice_date_due</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>invoice_origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>invoice_payment_term_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>invoice_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>invoice_incoterm_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>display_qr_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>qr_code_method</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>invoice_outstanding_credits_debits_widget</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>invoice_has_outstanding</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>invoice_payments_widget</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>invoice_vendor_bill_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>invoice_source_email</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>invoice_partner_display_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>invoice_cash_rounding_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>invoice_filter_type_domain</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>bank_partner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>invoice_has_matching_suspense_amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>tax_lock_date_message</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>display_inactive_currency_warning</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>tax_country_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>tax_country_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>has_reconciled_entries</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>show_reset_to_draft_button</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>restrict_mode_hash_table</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>secure_sequence_number</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>inalterable_hash</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>string_to_hash</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>__last_update</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>display_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>create_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>create_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>write_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>write_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>attachment_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>payment_state_before_switch</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>edi_document_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>edi_state</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>edi_error_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>edi_blocking_level</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>edi_error_message</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>edi_web_services_to_process</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>edi_show_cancel_button</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>edi_show_abandon_cancel_button</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>duplicated_vendor_ref</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>extract_state</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>extract_status_code</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>extract_error_message</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>extract_remote_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>extract_word_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>extract_can_show_resend_button</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>extract_can_show_send_button</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>transaction_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>authorized_transaction_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>amount_paid</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>purchase_vendor_bill_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>purchase_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>stock_move_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>stock_valuation_layer_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>transfer_model_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>tax_closing_end_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>tax_report_control_error</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>team_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>partner_shipping_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>asset_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>asset_asset_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>asset_remaining_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>asset_depreciated_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>asset_manually_modified</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>asset_value_change</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>asset_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>asset_ids_display_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>asset_id_display_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>number_asset_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>draft_asset_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>landed_costs_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>landed_costs_visible</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>manual_currency_rate_active</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>manual_currency_rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>third_party_account_payment</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>fiscal_provider</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>x_tasa</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>x_payment_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>exclude_xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>taxpayer</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>x_nota_entrega</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>sale_order_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>sale_order_number</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>amount_untaxed_rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>amount_tax_rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>amount_total_rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>x_nentrega</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>x_notaentrega</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>x_studio_total_</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>x_studio_deuda</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>x_nexpediente</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>x_nplanilla</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>x_ncomprobanteislr</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>x_tipodoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>x_ncomprobante</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>x_docafectado</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>x_noc</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>x_roc</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>x_ncontrol</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>x_retencionislr</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>x_studio_related_field_35Zlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>x_studio_orden_de_compra</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>x_retencion</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>move_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>move_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>parent_state</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>journal_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>company_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>company_currency_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>account_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>account_internal_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>account_internal_group</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>account_root_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>price_unit</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>debit</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>credit</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>balance</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>cumulated_balance</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>amount_currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>price_subtotal</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>price_total</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>reconciled</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>date_maturity</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>currency_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>partner_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>product_uom_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>product_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>product_uom_category_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>reconcile_model_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>payment_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>statement_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>statement_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>tax_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>group_tax_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>tax_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>tax_group_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>tax_base_amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>tax_repartition_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>tax_tag_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>tax_audit</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>tax_tag_invert</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>amount_residual</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>amount_residual_currency</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>full_reconcile_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>matched_debit_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>matched_credit_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>matching_number</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>analytic_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>analytic_account_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>analytic_tag_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>recompute_tax_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>display_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>is_rounding_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>exclude_from_invoice_tab</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>__last_update</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>display_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>create_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>create_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>write_uid</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>write_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>move_attachment_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>vehicle_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>need_vehicle</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>purchase_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>purchase_order_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>is_anglo_saxon_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>predict_from_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>expected_pay_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>internal_note</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>next_action_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>sale_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>asset_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>consolidation_journal_line_ids</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>followup_line_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>followup_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>product_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>is_landed_costs_line</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>non_deductible_tax_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>x_studio_many2one_field_FCO3N</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>x_studio_related_field_eOzzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>x_studio_many2one_field_BMZyG</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>x_studio_related_field_4zjYm</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>x_studio_fabricante</t>
         </is>
       </c>
     </row>
@@ -8354,7 +11507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A74"/>
+  <dimension ref="A1:A75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8877,6 +12030,13 @@
       <c r="A74" t="inlineStr">
         <is>
           <t>x_studio_sublinea</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>x_studio_fabricante</t>
         </is>
       </c>
     </row>

</xml_diff>